<commit_message>
updating regression analysis tables
</commit_message>
<xml_diff>
--- a/supplement/methods/goal_table.xlsx
+++ b/supplement/methods/goal_table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="4660" yWindow="0" windowWidth="19420" windowHeight="17460" tabRatio="500"/>
@@ -19,73 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
-  <si>
-    <t>Goal</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Food Provision</t>
-  </si>
-  <si>
-    <t>First Nations Resource Access Opportunities</t>
-  </si>
-  <si>
-    <t>Subgoal or Component</t>
-  </si>
-  <si>
-    <t>Ecosystem Services</t>
-  </si>
-  <si>
-    <t>Sense of Place</t>
-  </si>
-  <si>
-    <t>Livelihoods and Economies</t>
-  </si>
-  <si>
-    <t>Tourism and Recreation</t>
-  </si>
-  <si>
-    <t>Clean Waters</t>
-  </si>
-  <si>
-    <t>Biodiversity</t>
-  </si>
-  <si>
-    <t>Wild-capture fisheries</t>
-  </si>
-  <si>
-    <t>Mariculture</t>
-  </si>
-  <si>
-    <t>Salmon</t>
-  </si>
-  <si>
-    <t>Carbon Storage</t>
-  </si>
-  <si>
-    <t>Coastal Protection</t>
-  </si>
-  <si>
-    <t>Lasting Special Places</t>
-  </si>
-  <si>
-    <t>Iconic Species</t>
-  </si>
-  <si>
-    <t>Coastal Livelihoods</t>
-  </si>
-  <si>
-    <t>First Nations Livelihoods</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Habitats</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>All fisheries at B/BMSY of 1; all fisheries fished according to DFO harvest control rule; no fisheries data-limited</t>
   </si>
@@ -93,9 +27,6 @@
     <t>Finfish and shellfish harvests meet potential harvest based on tenure area and regional average growth potential index</t>
   </si>
   <si>
-    <t>All indicator stocks at escapement targets</t>
-  </si>
-  <si>
     <t>Herring spawn index: three-year running mean index at reference index value, calculated as mean index from 1940-1960; Shellfish closures: zero area-weighted average closure days due to sanitation, chemicals, or biotoxins; Salmon: all indicator stocks at or above escapement targets; First Nations commercial fishing licenses: proportion of licenses greater than or equal to proportion of First Nations population in region, with a floor of 15%</t>
   </si>
   <si>
@@ -130,6 +61,75 @@
   </si>
   <si>
     <t>Salt marsh extents at 1990 levels; zero trawl pressure on soft bottom habitat and ecologically/biologically significant areas (sponge reefs, deepwater corals, seamounts, hydrothermal vents)</t>
+  </si>
+  <si>
+    <t>Subgoal</t>
+  </si>
+  <si>
+    <t>Goal Name</t>
+  </si>
+  <si>
+    <t>Habitat Services (HS)</t>
+  </si>
+  <si>
+    <t>Food Provision (FP)</t>
+  </si>
+  <si>
+    <t>First Nations Resource Access Opportunities (AO)</t>
+  </si>
+  <si>
+    <t>Coastal Livelihoods (LV)</t>
+  </si>
+  <si>
+    <t>Tourism and Recreation (TR)</t>
+  </si>
+  <si>
+    <t>Sense of Place (SP)</t>
+  </si>
+  <si>
+    <t>Biodiversity (BD)</t>
+  </si>
+  <si>
+    <t>Clean Waters (CW)</t>
+  </si>
+  <si>
+    <t>Habitats (HAB)</t>
+  </si>
+  <si>
+    <t>Species (SPP)</t>
+  </si>
+  <si>
+    <t>Iconic Species (ICO)</t>
+  </si>
+  <si>
+    <t>Lasting Special Places (LSP)</t>
+  </si>
+  <si>
+    <t>non-First Nations Livelihoods (LVO)</t>
+  </si>
+  <si>
+    <t>First Nations Livelihoods (LVF)</t>
+  </si>
+  <si>
+    <t>Salmon (SAL)</t>
+  </si>
+  <si>
+    <t>Mariculture (MAR)</t>
+  </si>
+  <si>
+    <t>Wild-capture fisheries (FIS)</t>
+  </si>
+  <si>
+    <t>All indicator stocks at escapement targets and/or catch targets</t>
+  </si>
+  <si>
+    <t>Coastal Protection (CPP)</t>
+  </si>
+  <si>
+    <t>Carbon Storage (CSS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -142,7 +142,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -179,8 +179,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -190,9 +200,19 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,7 +545,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -536,145 +556,169 @@
     <col min="4" max="4" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="30">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="1" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="105">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="45">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45">
+      <c r="A9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30">
-      <c r="B3" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="45">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="105">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30">
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="45">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45">
-      <c r="B11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="45">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="45">
-      <c r="B15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update goal table columns
</commit_message>
<xml_diff>
--- a/supplement/methods/goal_table.xlsx
+++ b/supplement/methods/goal_table.xlsx
@@ -66,9 +66,6 @@
     <t>Subgoal</t>
   </si>
   <si>
-    <t>Goal Name</t>
-  </si>
-  <si>
     <t>Habitat Services (HS)</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Goal</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -558,7 +558,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>14</v>
@@ -569,10 +569,10 @@
     </row>
     <row r="2" spans="1:3" ht="30">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="3" spans="1:3" ht="30">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -591,10 +591,10 @@
     </row>
     <row r="4" spans="1:3" ht="30">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
@@ -602,10 +602,10 @@
     </row>
     <row r="5" spans="1:3" ht="30">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -613,21 +613,21 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="105">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
@@ -635,10 +635,10 @@
     </row>
     <row r="8" spans="1:3" ht="45">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -646,10 +646,10 @@
     </row>
     <row r="9" spans="1:3" ht="45">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -657,10 +657,10 @@
     </row>
     <row r="10" spans="1:3" ht="45">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -668,10 +668,10 @@
     </row>
     <row r="11" spans="1:3" ht="60">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -679,10 +679,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
@@ -690,10 +690,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="14" spans="1:3" ht="45">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -712,10 +712,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>10</v>

</xml_diff>